<commit_message>
before creating elg 2 and 3 subfile
</commit_message>
<xml_diff>
--- a/SPIN_Inverter_PIN_Mapping.xlsx
+++ b/SPIN_Inverter_PIN_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twalter\Local\Inverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0D8979-20A3-407D-A349-F64046172CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DF9BF3-A65C-460C-9BC9-BC897F6657BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10335776-0D9B-485B-BFEC-E4BDD3F10738}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>PIN number</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>HRTIM1_CHE2</t>
-  </si>
-  <si>
-    <t>VPhase3_sense</t>
   </si>
   <si>
     <t>VPhase2_sense</t>
@@ -774,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE2EDB6-F4C9-4E3F-9063-0CDA18A8B412}">
   <dimension ref="A1:AQ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -805,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -948,7 +945,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1014,7 +1011,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1124,7 +1121,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1135,7 +1132,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.35">
@@ -1146,7 +1143,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.35">
@@ -1157,7 +1154,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.35">
@@ -1179,7 +1176,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.35">
@@ -1190,7 +1187,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.35">
@@ -1212,7 +1209,7 @@
         <v>31</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.35">

</xml_diff>